<commit_message>
Consist updates, [747] WIP
</commit_message>
<xml_diff>
--- a/bugs.xlsx
+++ b/bugs.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D707E123-EFF7-4892-8167-DA4F693845E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2AE9C0-6BB4-4349-88DC-B3A89ACFBD9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="15247" windowHeight="11647" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1350" yWindow="2910" windowWidth="15248" windowHeight="11648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ZvNL" sheetId="1" r:id="rId1"/>
+    <sheet name="HSL" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,11 +26,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Tb1 uitrijder blijft rood
 Bug treedt niet op in leeg scenario zonder AI verkeer (moet wel restarten)
 Bug treedt niet op met AI Tba-Tb2</t>
+  </si>
+  <si>
+    <t>Shl1/2-Asra sein op rood, tab ok</t>
   </si>
 </sst>
 </file>
@@ -352,7 +356,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -369,4 +373,27 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBFFBECE-5A25-42A8-8389-74B5039D1A1B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="55.46484375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>